<commit_message>
Dates and values order
</commit_message>
<xml_diff>
--- a/test/test_df.xlsx
+++ b/test/test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A470222\Documents\Python Scripts\data_quality\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77637628-4BA0-4979-B18B-45423AE2A4BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360AC705-5CD9-4275-A47D-FB11D5395869}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>index</t>
   </si>
@@ -102,7 +102,31 @@
     <t>l</t>
   </si>
   <si>
-    <t>Value in column A not between 2020-01-01 and 2022-01-01</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Dates D, E, F are not in the correct order - Values G, H, I are not in the correct order</t>
+  </si>
+  <si>
+    <t>Value in column A not between 2020-01-01 and 2022-01-01 - Dates D, E, F are not in the correct order - Values G, H, I are not in the correct order</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -138,10 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,19 +481,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26F9433-4DCB-4F98-8509-33F4BD68965F}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,10 +509,28 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -498,8 +543,14 @@
       <c r="D2" s="1">
         <v>44197</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -512,11 +563,17 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -529,11 +586,21 @@
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>44197</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -543,8 +610,17 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>44197</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -554,11 +630,21 @@
       <c r="D6" s="1">
         <v>44389</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>15</v>
       </c>
@@ -568,11 +654,29 @@
       <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F7" s="1">
+        <v>44197</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44197</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -582,11 +686,24 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F8" s="1">
+        <v>44197</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -596,19 +713,49 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1">
+        <v>44197</v>
+      </c>
+      <c r="G9" s="1">
+        <v>44197</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>43831</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -618,8 +765,46 @@
       <c r="D11" s="1">
         <v>32874</v>
       </c>
-      <c r="E11" t="s">
-        <v>22</v>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>44197</v>
+      </c>
+      <c r="G11" s="1">
+        <v>43831</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3">
+        <v>2</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44197</v>
+      </c>
+      <c r="F12" s="1">
+        <v>43831</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Impala test + automatic datetime format
</commit_message>
<xml_diff>
--- a/test/test_df.xlsx
+++ b/test/test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A470222\Documents\Python Scripts\data_quality\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31930A2-A4B0-4FCF-BFCC-6140720317CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915F0701-DA2A-44CE-BC29-36A9F036F3A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" firstSheet="10" activeTab="17" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" firstSheet="7" activeTab="17" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="96">
   <si>
     <t>index</t>
   </si>
@@ -2271,7 +2271,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2315,8 +2315,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>33</v>
+      <c r="A4" s="4">
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>85</v>
@@ -2342,6 +2342,9 @@
       </c>
     </row>
     <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
@@ -2351,7 +2354,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>88</v>
@@ -2362,7 +2365,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>89</v>
@@ -2376,7 +2379,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>95</v>
@@ -2390,7 +2393,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
order dates dimension table
</commit_message>
<xml_diff>
--- a/test/test_df.xlsx
+++ b/test/test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A470222\Documents\Python Scripts\data_quality\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915F0701-DA2A-44CE-BC29-36A9F036F3A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A0871D-55D9-487A-B509-9037A62BE4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" firstSheet="7" activeTab="17" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" firstSheet="8" activeTab="19" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,8 @@
     <sheet name="custom_condition" sheetId="15" r:id="rId16"/>
     <sheet name="dimension_table" sheetId="17" r:id="rId17"/>
     <sheet name="fact_table" sheetId="18" r:id="rId18"/>
+    <sheet name="user_list" sheetId="19" r:id="rId19"/>
+    <sheet name="products" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="103">
   <si>
     <t>index</t>
   </si>
@@ -360,6 +362,27 @@
   </si>
   <si>
     <t>010</t>
+  </si>
+  <si>
+    <t>registration_date</t>
+  </si>
+  <si>
+    <t>2021-01-01</t>
+  </si>
+  <si>
+    <t>2021-01-02</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>selling_date</t>
+  </si>
+  <si>
+    <t>Dates selling_date, registration_date are not in the correct order</t>
   </si>
 </sst>
 </file>
@@ -2130,7 +2153,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2270,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647218C9-F641-4EBC-8F76-9B564D0F7D90}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2394,6 +2417,110 @@
     <row r="11" spans="1:4">
       <c r="A11">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial"&amp;8&amp;K000000INTERNAL&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE8B40A-2F02-46EA-9C9D-62E774A84988}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2510,6 +2637,147 @@
       </c>
       <c r="B11">
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial"&amp;8&amp;K000000INTERNAL&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACB48D-ECB1-4A5C-AED2-4F9C968DA995}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3260,7 +3528,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="A1:F11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
value order dimension table
</commit_message>
<xml_diff>
--- a/test/test_df.xlsx
+++ b/test/test_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A470222\Documents\Python Scripts\data_quality\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A0871D-55D9-487A-B509-9037A62BE4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E089BF8-5BA1-4C3D-A9FA-039B0CDB2051}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" firstSheet="8" activeTab="19" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="799" firstSheet="9" activeTab="20" xr2:uid="{95E7790A-81A8-4725-9CAF-8FDD23C80EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="fact_table" sheetId="18" r:id="rId18"/>
     <sheet name="user_list" sheetId="19" r:id="rId19"/>
     <sheet name="products" sheetId="20" r:id="rId20"/>
+    <sheet name="products2" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="106">
   <si>
     <t>index</t>
   </si>
@@ -383,6 +384,15 @@
   </si>
   <si>
     <t>Dates selling_date, registration_date are not in the correct order</t>
+  </si>
+  <si>
+    <t>max_products</t>
+  </si>
+  <si>
+    <t>n_products</t>
+  </si>
+  <si>
+    <t>Values n_products, max_products are not in the correct order</t>
   </si>
 </sst>
 </file>
@@ -441,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -454,6 +464,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1930,7 +1943,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2430,66 +2443,85 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE8B40A-2F02-46EA-9C9D-62E774A84988}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>72</v>
       </c>
       <c r="B1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2497,7 +2529,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2505,22 +2537,31 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="B11" s="2" t="s">
         <v>98</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2652,14 +2693,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ACB48D-ECB1-4A5C-AED2-4F9C968DA995}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2778,6 +2819,145 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Arial"&amp;8&amp;K000000INTERNAL&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012A182E-6C46-4A39-B04A-4A02F1058509}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10">
+        <v>200</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>